<commit_message>
Optimized dataprovider, removed Depends on from test methods
</commit_message>
<xml_diff>
--- a/DataDriven_Core_framework/Data.xlsx
+++ b/DataDriven_Core_framework/Data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17927"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -246,7 +246,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -381,7 +381,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -414,26 +414,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -466,23 +449,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -661,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,7 +754,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>41</v>

</xml_diff>